<commit_message>
Added event calculation and some ordering
</commit_message>
<xml_diff>
--- a/docs/probabilities/data_minimization.xlsx
+++ b/docs/probabilities/data_minimization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/work/git/cportugalz/pucp_gpu/docs/probabilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCA33AC-9C66-0343-88DE-A4DE1B10F35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37F8832-A066-6E4E-9DD0-58A72CEC7668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="54">
   <si>
     <t>Parámetros fijos:</t>
   </si>
@@ -486,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -541,14 +541,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -559,9 +554,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,8 +604,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="Rectángulo 3">
@@ -850,7 +860,7 @@
                     </m:oMathPara>
                   </a14:m>
                 </mc:Choice>
-                <mc:Fallback xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns=""/>
+                <mc:Fallback xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math"/>
               </mc:AlternateContent>
               <a:endParaRPr sz="1100">
                 <a:latin typeface="Cambria Math"/>
@@ -861,7 +871,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="Rectángulo 3">
@@ -1083,8 +1093,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>276223</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="Rectángulo 4">
@@ -1339,7 +1349,7 @@
                     </m:oMathPara>
                   </a14:m>
                 </mc:Choice>
-                <mc:Fallback xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns=""/>
+                <mc:Fallback xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math"/>
               </mc:AlternateContent>
               <a:endParaRPr sz="1100">
                 <a:latin typeface="Cambria Math"/>
@@ -1350,7 +1360,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="Rectángulo 4">
@@ -1572,8 +1582,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>266697</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="Rectángulo 5">
@@ -1828,7 +1838,7 @@
                     </m:oMathPara>
                   </a14:m>
                 </mc:Choice>
-                <mc:Fallback xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns=""/>
+                <mc:Fallback xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math"/>
               </mc:AlternateContent>
               <a:endParaRPr sz="1100">
                 <a:latin typeface="Cambria Math"/>
@@ -1839,7 +1849,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="Rectángulo 5">
@@ -2061,8 +2071,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>257171</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="Rectángulo 6">
@@ -2317,7 +2327,7 @@
                     </m:oMathPara>
                   </a14:m>
                 </mc:Choice>
-                <mc:Fallback xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns=""/>
+                <mc:Fallback xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math"/>
               </mc:AlternateContent>
               <a:endParaRPr sz="1100">
                 <a:latin typeface="Cambria Math"/>
@@ -2328,7 +2338,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="Rectángulo 6">
@@ -2600,14 +2610,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1186457</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>294408</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>13193</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>152395</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>284881</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3666</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -2624,8 +2634,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="1796057" y="1904133"/>
-              <a:ext cx="4442812" cy="285747"/>
+              <a:off x="1857743" y="1936336"/>
+              <a:ext cx="5080081" cy="280759"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3096,7 +3106,7 @@
                     </m:oMathPara>
                   </a14:m>
                 </mc:Choice>
-                <mc:Fallback xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns=""/>
+                <mc:Fallback xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math"/>
               </mc:AlternateContent>
               <a:endParaRPr sz="1100">
                 <a:latin typeface="Cambria Math"/>
@@ -3121,8 +3131,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="1796057" y="1904133"/>
-              <a:ext cx="4442812" cy="285747"/>
+              <a:off x="1857743" y="1936336"/>
+              <a:ext cx="5080081" cy="280759"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3177,7 +3187,7 @@
                 <a:t> </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="es-MX" i="0">
+                <a:rPr lang="en-US" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>(</a:t>
@@ -3263,7 +3273,7 @@
                 <a:t> </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="es-MX" sz="1200" i="0">
+                <a:rPr lang="en-US" sz="1200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>(</a:t>
@@ -3349,7 +3359,7 @@
                 <a:t> </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="es-MX" sz="1200" i="0">
+                <a:rPr lang="en-US" sz="1200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>(</a:t>
@@ -3435,7 +3445,7 @@
                 <a:t> </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="es-MX" sz="1200" i="0">
+                <a:rPr lang="en-US" sz="1200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>(</a:t>
@@ -3521,7 +3531,7 @@
                 <a:t> </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="es-MX" sz="1200" i="0">
+                <a:rPr lang="en-US" sz="1200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>(</a:t>
@@ -3785,8 +3795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3802,19 +3812,19 @@
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="29"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C3" s="3">
         <v>1300</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="35">
         <v>0.197327</v>
       </c>
-      <c r="E3" s="30"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="5" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
@@ -3851,13 +3861,13 @@
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
@@ -3888,7 +3898,7 @@
       <c r="E16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="40" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="14" t="s">
@@ -3903,7 +3913,7 @@
       <c r="J16" s="15"/>
       <c r="K16" s="16"/>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:23" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
@@ -3929,6 +3939,9 @@
         <v>3.9999999999999997E-24</v>
       </c>
       <c r="J17" s="11"/>
+      <c r="M17" s="29" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B18" s="12"/>
@@ -3942,6 +3955,50 @@
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
+      <c r="M18" s="38">
+        <f>SUM(N18:W18)</f>
+        <v>1.6767609261574992</v>
+      </c>
+      <c r="N18">
+        <f>(N$27-C$21)^2/C$21</f>
+        <v>2.8196311603442856E-3</v>
+      </c>
+      <c r="O18" s="20">
+        <f>(O$27-D$21)^2/D$21</f>
+        <v>4.8959184022726712E-2</v>
+      </c>
+      <c r="P18" s="20">
+        <f>(P$27-E$21)^2/E$21</f>
+        <v>2.9965319901240711E-2</v>
+      </c>
+      <c r="Q18" s="20">
+        <f>(Q$27-F$21)^2/F$21</f>
+        <v>3.7399536363471854E-2</v>
+      </c>
+      <c r="R18" s="20">
+        <f>(R$27-G$21)^2/G$21</f>
+        <v>0.13085627883813372</v>
+      </c>
+      <c r="S18" s="20">
+        <f>(S$27-H$21)^2/H$21</f>
+        <v>9.4274273332027703E-2</v>
+      </c>
+      <c r="T18" s="20">
+        <f>(T$27-I$21)^2/I$21</f>
+        <v>1.92103092783509E-2</v>
+      </c>
+      <c r="U18" s="20">
+        <f>(U$27-J$21)^2/J$21</f>
+        <v>5.9331300999036279E-3</v>
+      </c>
+      <c r="V18" s="20">
+        <f>(V$27-K$21)^2/K$21</f>
+        <v>0.29433124400577038</v>
+      </c>
+      <c r="W18" s="20">
+        <f>(W$27-L$21)^2/L$21</f>
+        <v>1.0130120191555292</v>
+      </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
@@ -3977,7 +4034,50 @@
       <c r="L19" s="19">
         <v>10</v>
       </c>
-      <c r="N19" s="20"/>
+      <c r="M19" s="38">
+        <f>SUM(N19:W19)</f>
+        <v>1.276610900370859</v>
+      </c>
+      <c r="N19" s="20">
+        <f>(N$28-C$21)^2/C$21</f>
+        <v>6.0178735128879144E-3</v>
+      </c>
+      <c r="O19" s="20">
+        <f>(O$28-D$21)^2/D$21</f>
+        <v>5.9096606369688366E-2</v>
+      </c>
+      <c r="P19" s="20">
+        <f>(P$28-E$21)^2/E$21</f>
+        <v>9.4059270887313744E-3</v>
+      </c>
+      <c r="Q19" s="20">
+        <f>(Q$28-F$21)^2/F$21</f>
+        <v>3.243578211497981E-3</v>
+      </c>
+      <c r="R19" s="20">
+        <f>(R$28-G$21)^2/G$21</f>
+        <v>5.221614875527221E-2</v>
+      </c>
+      <c r="S19" s="20">
+        <f>(S$28-H$21)^2/H$21</f>
+        <v>8.9456564176106285E-2</v>
+      </c>
+      <c r="T19" s="20">
+        <f>(T$28-I$21)^2/I$21</f>
+        <v>4.2444262953541326E-2</v>
+      </c>
+      <c r="U19" s="20">
+        <f>(U$28-J$21)^2/J$21</f>
+        <v>6.9858557981370036E-4</v>
+      </c>
+      <c r="V19" s="20">
+        <f>(V$28-K$21)^2/K$21</f>
+        <v>0.1833965216471965</v>
+      </c>
+      <c r="W19" s="20">
+        <f>(W$28-L$21)^2/L$21</f>
+        <v>0.83063483207612321</v>
+      </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
@@ -4013,6 +4113,50 @@
       <c r="L20" s="17">
         <v>6</v>
       </c>
+      <c r="M20" s="38">
+        <f t="shared" ref="M20:M21" si="0">SUM(N20:W20)</f>
+        <v>1.8556161982886241</v>
+      </c>
+      <c r="N20" s="20">
+        <f>(N$29-C$21)^2/C$21</f>
+        <v>1.7767040013110574E-3</v>
+      </c>
+      <c r="O20" s="20">
+        <f>(O$29-D$21)^2/D$21</f>
+        <v>5.726703232762323E-2</v>
+      </c>
+      <c r="P20" s="20">
+        <f>(P$29-E$21)^2/E$21</f>
+        <v>3.3381968787149649E-2</v>
+      </c>
+      <c r="Q20" s="20">
+        <f>(Q$29-F$21)^2/F$21</f>
+        <v>3.7610195174075274E-2</v>
+      </c>
+      <c r="R20" s="20">
+        <f>(R$29-G$21)^2/G$21</f>
+        <v>0.11828420225244941</v>
+      </c>
+      <c r="S20" s="20">
+        <f>(S$29-H$21)^2/H$21</f>
+        <v>7.1321806040773594E-2</v>
+      </c>
+      <c r="T20" s="20">
+        <f>(T$29-I$21)^2/I$21</f>
+        <v>6.9375016735841568E-3</v>
+      </c>
+      <c r="U20" s="20">
+        <f>(U$29-J$21)^2/J$21</f>
+        <v>1.9729197321824751E-2</v>
+      </c>
+      <c r="V20" s="20">
+        <f>(V$29-K$21)^2/K$21</f>
+        <v>0.37046055324387034</v>
+      </c>
+      <c r="W20" s="20">
+        <f>(W$29-L$21)^2/L$21</f>
+        <v>1.1388470374659627</v>
+      </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
@@ -4048,6 +4192,50 @@
       <c r="L21" s="17">
         <v>127.79600000000001</v>
       </c>
+      <c r="M21" s="38">
+        <f t="shared" si="0"/>
+        <v>1.4559597742053965</v>
+      </c>
+      <c r="N21" s="20">
+        <f>(N$30-C$21)^2/C$21</f>
+        <v>1.5888938395275378E-3</v>
+      </c>
+      <c r="O21" s="20">
+        <f>(O$30-D$21)^2/D$21</f>
+        <v>2.3522358941009396E-2</v>
+      </c>
+      <c r="P21" s="20">
+        <f>(P$30-E$21)^2/E$21</f>
+        <v>1.8025451885268641E-2</v>
+      </c>
+      <c r="Q21" s="20">
+        <f>(Q$30-F$21)^2/F$21</f>
+        <v>2.5370214975221482E-4</v>
+      </c>
+      <c r="R21" s="20">
+        <f>(R$30-G$21)^2/G$21</f>
+        <v>8.2275064051409261E-2</v>
+      </c>
+      <c r="S21" s="20">
+        <f>(S$30-H$21)^2/H$21</f>
+        <v>9.1753296144443164E-2</v>
+      </c>
+      <c r="T21" s="20">
+        <f>(T$30-I$21)^2/I$21</f>
+        <v>2.7668288927567702E-2</v>
+      </c>
+      <c r="U21" s="20">
+        <f>(U$30-J$21)^2/J$21</f>
+        <v>1.4575427529447352E-3</v>
+      </c>
+      <c r="V21" s="20">
+        <f>(V$30-K$21)^2/K$21</f>
+        <v>0.25483111184950902</v>
+      </c>
+      <c r="W21" s="20">
+        <f>(W$30-L$21)^2/L$21</f>
+        <v>0.95458406366396475</v>
+      </c>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="s">
@@ -4055,16 +4243,6 @@
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="20"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="13"/>
-      <c r="W24" s="13"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B25" s="12"/>
@@ -4075,28 +4253,28 @@
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
-      <c r="J25" s="36" t="s">
+      <c r="J25" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="K25" s="36" t="s">
+      <c r="K25" s="30" t="s">
         <v>52</v>
       </c>
       <c r="L25" s="13" t="s">
         <v>51</v>
       </c>
       <c r="M25" s="21"/>
-      <c r="N25" s="32" t="s">
+      <c r="N25" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="33"/>
-      <c r="V25" s="33"/>
-      <c r="W25" s="34"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="33"/>
     </row>
     <row r="26" spans="2:23" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="14" t="s">
@@ -4616,18 +4794,18 @@
       <c r="E44" s="20"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="N45" s="35" t="s">
+      <c r="N45" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="O45" s="35"/>
-      <c r="P45" s="35"/>
-      <c r="Q45" s="35"/>
-      <c r="R45" s="35"/>
-      <c r="S45" s="35"/>
-      <c r="T45" s="35"/>
-      <c r="U45" s="35"/>
-      <c r="V45" s="35"/>
-      <c r="W45" s="35"/>
+      <c r="O45" s="37"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="37"/>
+      <c r="V45" s="37"/>
+      <c r="W45" s="37"/>
     </row>
     <row r="46" spans="2:23" ht="17" x14ac:dyDescent="0.2">
       <c r="B46" s="14" t="s">
@@ -5211,18 +5389,18 @@
       <c r="K65" s="13"/>
       <c r="L65" s="13"/>
       <c r="M65" s="21"/>
-      <c r="N65" s="32" t="s">
+      <c r="N65" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="O65" s="33"/>
-      <c r="P65" s="33"/>
-      <c r="Q65" s="33"/>
-      <c r="R65" s="33"/>
-      <c r="S65" s="33"/>
-      <c r="T65" s="33"/>
-      <c r="U65" s="33"/>
-      <c r="V65" s="33"/>
-      <c r="W65" s="34"/>
+      <c r="O65" s="32"/>
+      <c r="P65" s="32"/>
+      <c r="Q65" s="32"/>
+      <c r="R65" s="32"/>
+      <c r="S65" s="32"/>
+      <c r="T65" s="32"/>
+      <c r="U65" s="32"/>
+      <c r="V65" s="32"/>
+      <c r="W65" s="33"/>
     </row>
     <row r="66" spans="2:23" ht="17" x14ac:dyDescent="0.2">
       <c r="B66" s="14" t="s">

</xml_diff>